<commit_message>
Updating documentation for next checkoff
</commit_message>
<xml_diff>
--- a/Documentation/Time.xlsx
+++ b/Documentation/Time.xlsx
@@ -119,9 +119,6 @@
     <t>Thurs 1/30</t>
   </si>
   <si>
-    <t>Week 5</t>
-  </si>
-  <si>
     <t>Fri 2/1</t>
   </si>
   <si>
@@ -141,6 +138,9 @@
   </si>
   <si>
     <t>Thurs 2/7</t>
+  </si>
+  <si>
+    <t>Week 0</t>
   </si>
 </sst>
 </file>
@@ -460,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,7 +476,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -516,7 +516,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -583,139 +583,208 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <f>SUM(B9:B16)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <f>SUM(B19:B26)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <f>SUM(B29:B36)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>